<commit_message>
Ride Finished And Sound System Finished
</commit_message>
<xml_diff>
--- a/Src/Data/Tables/ItemDefine.xlsx
+++ b/Src/Data/Tables/ItemDefine.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="191">
   <si>
     <t>描述</t>
   </si>
@@ -551,6 +551,39 @@
   </si>
   <si>
     <t>UI/ItemIcons/equip3017</t>
+  </si>
+  <si>
+    <t>Tiger Of Iceberg</t>
+  </si>
+  <si>
+    <t>Its feather looks nice.</t>
+  </si>
+  <si>
+    <t>RIDE</t>
+  </si>
+  <si>
+    <t>Ride</t>
+  </si>
+  <si>
+    <t>UI/ItemIcons/ride8001</t>
+  </si>
+  <si>
+    <t>Beast Of Nightmare</t>
+  </si>
+  <si>
+    <t>Our best recommandation is to stay indoor during night.(From adventurers who were teared apart by these big cats coming out late night)</t>
+  </si>
+  <si>
+    <t>UI/ItemIcons/ride8002</t>
+  </si>
+  <si>
+    <t>Big Cat</t>
+  </si>
+  <si>
+    <t>After all, a cat.</t>
+  </si>
+  <si>
+    <t>UI/ItemIcons/ride8003</t>
   </si>
 </sst>
 </file>
@@ -626,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -719,6 +752,37 @@
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -768,7 +832,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A3:Q55" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A3:Q58" displayName="Table_1" id="1">
   <tableColumns count="17">
     <tableColumn name="Key" id="1"/>
     <tableColumn name="ID" id="2"/>
@@ -4062,22 +4126,45 @@
       <c r="AD55" s="1"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
+      <c r="A56" s="32">
+        <v>8001.0</v>
+      </c>
+      <c r="B56" s="32">
+        <v>8001.0</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="D56" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="E56" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="F56" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="G56" s="37">
+        <v>1.0</v>
+      </c>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="40">
+        <v>1000.0</v>
+      </c>
+      <c r="L56" s="40">
+        <v>500.0</v>
+      </c>
+      <c r="M56" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="N56" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="O56" s="39"/>
+      <c r="P56" s="41"/>
+      <c r="Q56" s="41"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
@@ -4093,22 +4180,45 @@
       <c r="AD56" s="1"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
+      <c r="A57" s="32">
+        <v>8002.0</v>
+      </c>
+      <c r="B57" s="32">
+        <v>8002.0</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="E57" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="F57" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="G57" s="37">
+        <v>1.0</v>
+      </c>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="40">
+        <v>1000.0</v>
+      </c>
+      <c r="L57" s="40">
+        <v>500.0</v>
+      </c>
+      <c r="M57" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="N57" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="O57" s="39"/>
+      <c r="P57" s="41"/>
+      <c r="Q57" s="41"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
@@ -4124,22 +4234,45 @@
       <c r="AD57" s="1"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
+      <c r="A58" s="32">
+        <v>8003.0</v>
+      </c>
+      <c r="B58" s="32">
+        <v>8003.0</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="E58" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="G58" s="37">
+        <v>1.0</v>
+      </c>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="40">
+        <v>1000.0</v>
+      </c>
+      <c r="L58" s="40">
+        <v>500.0</v>
+      </c>
+      <c r="M58" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="N58" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="O58" s="39"/>
+      <c r="P58" s="41"/>
+      <c r="Q58" s="41"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
@@ -4160,9 +4293,9 @@
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="43"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -4191,9 +4324,9 @@
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -4222,9 +4355,9 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="32"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="43"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
@@ -4253,9 +4386,9 @@
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="32"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="43"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -4284,9 +4417,9 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
-      <c r="G63" s="32"/>
-      <c r="H63" s="32"/>
-      <c r="I63" s="32"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="43"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -4315,9 +4448,9 @@
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
-      <c r="G64" s="32"/>
-      <c r="H64" s="32"/>
-      <c r="I64" s="32"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="43"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
@@ -4346,9 +4479,9 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
-      <c r="G65" s="32"/>
-      <c r="H65" s="32"/>
-      <c r="I65" s="32"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+      <c r="I65" s="43"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -4377,9 +4510,9 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="32"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="43"/>
+      <c r="I66" s="43"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
@@ -4408,9 +4541,9 @@
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
-      <c r="G67" s="32"/>
-      <c r="H67" s="32"/>
-      <c r="I67" s="32"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="43"/>
+      <c r="I67" s="43"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -4439,9 +4572,9 @@
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
-      <c r="G68" s="32"/>
-      <c r="H68" s="32"/>
-      <c r="I68" s="32"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="43"/>
+      <c r="I68" s="43"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
@@ -4470,9 +4603,9 @@
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="32"/>
-      <c r="I69" s="32"/>
+      <c r="G69" s="43"/>
+      <c r="H69" s="43"/>
+      <c r="I69" s="43"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
@@ -4501,9 +4634,9 @@
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
-      <c r="G70" s="32"/>
-      <c r="H70" s="32"/>
-      <c r="I70" s="32"/>
+      <c r="G70" s="43"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="43"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -4532,9 +4665,9 @@
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="32"/>
-      <c r="I71" s="32"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="43"/>
+      <c r="I71" s="43"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -4563,9 +4696,9 @@
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="32"/>
-      <c r="I72" s="32"/>
+      <c r="G72" s="43"/>
+      <c r="H72" s="43"/>
+      <c r="I72" s="43"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -4594,9 +4727,9 @@
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="32"/>
-      <c r="I73" s="32"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="43"/>
+      <c r="I73" s="43"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
@@ -4625,9 +4758,9 @@
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
-      <c r="G74" s="32"/>
-      <c r="H74" s="32"/>
-      <c r="I74" s="32"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="43"/>
+      <c r="I74" s="43"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
@@ -4656,9 +4789,9 @@
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
-      <c r="G75" s="32"/>
-      <c r="H75" s="32"/>
-      <c r="I75" s="32"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="43"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
@@ -4687,9 +4820,9 @@
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
-      <c r="G76" s="32"/>
-      <c r="H76" s="32"/>
-      <c r="I76" s="32"/>
+      <c r="G76" s="43"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="43"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
@@ -4718,9 +4851,9 @@
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
-      <c r="G77" s="32"/>
-      <c r="H77" s="32"/>
-      <c r="I77" s="32"/>
+      <c r="G77" s="43"/>
+      <c r="H77" s="43"/>
+      <c r="I77" s="43"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
@@ -4749,9 +4882,9 @@
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
-      <c r="G78" s="32"/>
-      <c r="H78" s="32"/>
-      <c r="I78" s="32"/>
+      <c r="G78" s="43"/>
+      <c r="H78" s="43"/>
+      <c r="I78" s="43"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
@@ -4780,9 +4913,9 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
-      <c r="G79" s="32"/>
-      <c r="H79" s="32"/>
-      <c r="I79" s="32"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="43"/>
+      <c r="I79" s="43"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
@@ -4811,9 +4944,9 @@
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
-      <c r="G80" s="32"/>
-      <c r="H80" s="32"/>
-      <c r="I80" s="32"/>
+      <c r="G80" s="43"/>
+      <c r="H80" s="43"/>
+      <c r="I80" s="43"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
@@ -4842,9 +4975,9 @@
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
-      <c r="G81" s="32"/>
-      <c r="H81" s="32"/>
-      <c r="I81" s="32"/>
+      <c r="G81" s="43"/>
+      <c r="H81" s="43"/>
+      <c r="I81" s="43"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
@@ -4873,9 +5006,9 @@
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
-      <c r="G82" s="32"/>
-      <c r="H82" s="32"/>
-      <c r="I82" s="32"/>
+      <c r="G82" s="43"/>
+      <c r="H82" s="43"/>
+      <c r="I82" s="43"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -4904,9 +5037,9 @@
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
-      <c r="G83" s="32"/>
-      <c r="H83" s="32"/>
-      <c r="I83" s="32"/>
+      <c r="G83" s="43"/>
+      <c r="H83" s="43"/>
+      <c r="I83" s="43"/>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
@@ -4935,9 +5068,9 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
-      <c r="G84" s="32"/>
-      <c r="H84" s="32"/>
-      <c r="I84" s="32"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="43"/>
+      <c r="I84" s="43"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
@@ -4966,9 +5099,9 @@
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
-      <c r="G85" s="32"/>
-      <c r="H85" s="32"/>
-      <c r="I85" s="32"/>
+      <c r="G85" s="43"/>
+      <c r="H85" s="43"/>
+      <c r="I85" s="43"/>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
@@ -4997,9 +5130,9 @@
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
-      <c r="G86" s="32"/>
-      <c r="H86" s="32"/>
-      <c r="I86" s="32"/>
+      <c r="G86" s="43"/>
+      <c r="H86" s="43"/>
+      <c r="I86" s="43"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
@@ -5028,9 +5161,9 @@
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
-      <c r="G87" s="32"/>
-      <c r="H87" s="32"/>
-      <c r="I87" s="32"/>
+      <c r="G87" s="43"/>
+      <c r="H87" s="43"/>
+      <c r="I87" s="43"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
@@ -5059,9 +5192,9 @@
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
-      <c r="G88" s="32"/>
-      <c r="H88" s="32"/>
-      <c r="I88" s="32"/>
+      <c r="G88" s="43"/>
+      <c r="H88" s="43"/>
+      <c r="I88" s="43"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
@@ -5090,9 +5223,9 @@
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
-      <c r="G89" s="32"/>
-      <c r="H89" s="32"/>
-      <c r="I89" s="32"/>
+      <c r="G89" s="43"/>
+      <c r="H89" s="43"/>
+      <c r="I89" s="43"/>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
@@ -5121,9 +5254,9 @@
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
-      <c r="G90" s="32"/>
-      <c r="H90" s="32"/>
-      <c r="I90" s="32"/>
+      <c r="G90" s="43"/>
+      <c r="H90" s="43"/>
+      <c r="I90" s="43"/>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
@@ -5152,9 +5285,9 @@
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
-      <c r="G91" s="32"/>
-      <c r="H91" s="32"/>
-      <c r="I91" s="32"/>
+      <c r="G91" s="43"/>
+      <c r="H91" s="43"/>
+      <c r="I91" s="43"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
@@ -5183,9 +5316,9 @@
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
-      <c r="G92" s="32"/>
-      <c r="H92" s="32"/>
-      <c r="I92" s="32"/>
+      <c r="G92" s="43"/>
+      <c r="H92" s="43"/>
+      <c r="I92" s="43"/>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
@@ -5214,9 +5347,9 @@
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
-      <c r="G93" s="32"/>
-      <c r="H93" s="32"/>
-      <c r="I93" s="32"/>
+      <c r="G93" s="43"/>
+      <c r="H93" s="43"/>
+      <c r="I93" s="43"/>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
@@ -5245,9 +5378,9 @@
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
-      <c r="G94" s="32"/>
-      <c r="H94" s="32"/>
-      <c r="I94" s="32"/>
+      <c r="G94" s="43"/>
+      <c r="H94" s="43"/>
+      <c r="I94" s="43"/>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
@@ -5276,9 +5409,9 @@
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
-      <c r="G95" s="32"/>
-      <c r="H95" s="32"/>
-      <c r="I95" s="32"/>
+      <c r="G95" s="43"/>
+      <c r="H95" s="43"/>
+      <c r="I95" s="43"/>
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
@@ -5307,9 +5440,9 @@
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
-      <c r="G96" s="32"/>
-      <c r="H96" s="32"/>
-      <c r="I96" s="32"/>
+      <c r="G96" s="43"/>
+      <c r="H96" s="43"/>
+      <c r="I96" s="43"/>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
@@ -5338,9 +5471,9 @@
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
-      <c r="G97" s="32"/>
-      <c r="H97" s="32"/>
-      <c r="I97" s="32"/>
+      <c r="G97" s="43"/>
+      <c r="H97" s="43"/>
+      <c r="I97" s="43"/>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
@@ -5369,9 +5502,9 @@
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
-      <c r="G98" s="32"/>
-      <c r="H98" s="32"/>
-      <c r="I98" s="32"/>
+      <c r="G98" s="43"/>
+      <c r="H98" s="43"/>
+      <c r="I98" s="43"/>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
@@ -5400,9 +5533,9 @@
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
-      <c r="G99" s="32"/>
-      <c r="H99" s="32"/>
-      <c r="I99" s="32"/>
+      <c r="G99" s="43"/>
+      <c r="H99" s="43"/>
+      <c r="I99" s="43"/>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
@@ -5431,9 +5564,9 @@
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
-      <c r="G100" s="32"/>
-      <c r="H100" s="32"/>
-      <c r="I100" s="32"/>
+      <c r="G100" s="43"/>
+      <c r="H100" s="43"/>
+      <c r="I100" s="43"/>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
@@ -5462,9 +5595,9 @@
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
-      <c r="G101" s="32"/>
-      <c r="H101" s="32"/>
-      <c r="I101" s="32"/>
+      <c r="G101" s="43"/>
+      <c r="H101" s="43"/>
+      <c r="I101" s="43"/>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
@@ -5493,9 +5626,9 @@
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
-      <c r="G102" s="32"/>
-      <c r="H102" s="32"/>
-      <c r="I102" s="32"/>
+      <c r="G102" s="43"/>
+      <c r="H102" s="43"/>
+      <c r="I102" s="43"/>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
@@ -5524,9 +5657,9 @@
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
-      <c r="G103" s="32"/>
-      <c r="H103" s="32"/>
-      <c r="I103" s="32"/>
+      <c r="G103" s="43"/>
+      <c r="H103" s="43"/>
+      <c r="I103" s="43"/>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
@@ -5555,9 +5688,9 @@
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
       <c r="E104" s="5"/>
-      <c r="G104" s="32"/>
-      <c r="H104" s="32"/>
-      <c r="I104" s="32"/>
+      <c r="G104" s="43"/>
+      <c r="H104" s="43"/>
+      <c r="I104" s="43"/>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
@@ -5586,9 +5719,9 @@
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
-      <c r="G105" s="32"/>
-      <c r="H105" s="32"/>
-      <c r="I105" s="32"/>
+      <c r="G105" s="43"/>
+      <c r="H105" s="43"/>
+      <c r="I105" s="43"/>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
@@ -5617,9 +5750,9 @@
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
-      <c r="G106" s="32"/>
-      <c r="H106" s="32"/>
-      <c r="I106" s="32"/>
+      <c r="G106" s="43"/>
+      <c r="H106" s="43"/>
+      <c r="I106" s="43"/>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
@@ -5648,9 +5781,9 @@
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
       <c r="E107" s="5"/>
-      <c r="G107" s="32"/>
-      <c r="H107" s="32"/>
-      <c r="I107" s="32"/>
+      <c r="G107" s="43"/>
+      <c r="H107" s="43"/>
+      <c r="I107" s="43"/>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
@@ -5679,9 +5812,9 @@
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
       <c r="E108" s="5"/>
-      <c r="G108" s="32"/>
-      <c r="H108" s="32"/>
-      <c r="I108" s="32"/>
+      <c r="G108" s="43"/>
+      <c r="H108" s="43"/>
+      <c r="I108" s="43"/>
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
@@ -5710,9 +5843,9 @@
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
-      <c r="G109" s="32"/>
-      <c r="H109" s="32"/>
-      <c r="I109" s="32"/>
+      <c r="G109" s="43"/>
+      <c r="H109" s="43"/>
+      <c r="I109" s="43"/>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
@@ -5741,9 +5874,9 @@
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5"/>
-      <c r="G110" s="32"/>
-      <c r="H110" s="32"/>
-      <c r="I110" s="32"/>
+      <c r="G110" s="43"/>
+      <c r="H110" s="43"/>
+      <c r="I110" s="43"/>
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
@@ -5772,9 +5905,9 @@
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
-      <c r="G111" s="32"/>
-      <c r="H111" s="32"/>
-      <c r="I111" s="32"/>
+      <c r="G111" s="43"/>
+      <c r="H111" s="43"/>
+      <c r="I111" s="43"/>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
@@ -5803,9 +5936,9 @@
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
       <c r="E112" s="5"/>
-      <c r="G112" s="32"/>
-      <c r="H112" s="32"/>
-      <c r="I112" s="32"/>
+      <c r="G112" s="43"/>
+      <c r="H112" s="43"/>
+      <c r="I112" s="43"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
@@ -5834,9 +5967,9 @@
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
-      <c r="G113" s="32"/>
-      <c r="H113" s="32"/>
-      <c r="I113" s="32"/>
+      <c r="G113" s="43"/>
+      <c r="H113" s="43"/>
+      <c r="I113" s="43"/>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
@@ -5865,9 +5998,9 @@
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
-      <c r="G114" s="32"/>
-      <c r="H114" s="32"/>
-      <c r="I114" s="32"/>
+      <c r="G114" s="43"/>
+      <c r="H114" s="43"/>
+      <c r="I114" s="43"/>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
@@ -5896,9 +6029,9 @@
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
       <c r="E115" s="5"/>
-      <c r="G115" s="32"/>
-      <c r="H115" s="32"/>
-      <c r="I115" s="32"/>
+      <c r="G115" s="43"/>
+      <c r="H115" s="43"/>
+      <c r="I115" s="43"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
@@ -5927,9 +6060,9 @@
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
       <c r="E116" s="5"/>
-      <c r="G116" s="32"/>
-      <c r="H116" s="32"/>
-      <c r="I116" s="32"/>
+      <c r="G116" s="43"/>
+      <c r="H116" s="43"/>
+      <c r="I116" s="43"/>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
@@ -5958,9 +6091,9 @@
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
       <c r="E117" s="5"/>
-      <c r="G117" s="32"/>
-      <c r="H117" s="32"/>
-      <c r="I117" s="32"/>
+      <c r="G117" s="43"/>
+      <c r="H117" s="43"/>
+      <c r="I117" s="43"/>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
@@ -5989,9 +6122,9 @@
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
-      <c r="G118" s="32"/>
-      <c r="H118" s="32"/>
-      <c r="I118" s="32"/>
+      <c r="G118" s="43"/>
+      <c r="H118" s="43"/>
+      <c r="I118" s="43"/>
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
@@ -6020,9 +6153,9 @@
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
       <c r="E119" s="5"/>
-      <c r="G119" s="32"/>
-      <c r="H119" s="32"/>
-      <c r="I119" s="32"/>
+      <c r="G119" s="43"/>
+      <c r="H119" s="43"/>
+      <c r="I119" s="43"/>
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
@@ -6051,9 +6184,9 @@
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
-      <c r="G120" s="32"/>
-      <c r="H120" s="32"/>
-      <c r="I120" s="32"/>
+      <c r="G120" s="43"/>
+      <c r="H120" s="43"/>
+      <c r="I120" s="43"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
@@ -6082,9 +6215,9 @@
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
-      <c r="G121" s="32"/>
-      <c r="H121" s="32"/>
-      <c r="I121" s="32"/>
+      <c r="G121" s="43"/>
+      <c r="H121" s="43"/>
+      <c r="I121" s="43"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
@@ -6113,9 +6246,9 @@
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
-      <c r="G122" s="32"/>
-      <c r="H122" s="32"/>
-      <c r="I122" s="32"/>
+      <c r="G122" s="43"/>
+      <c r="H122" s="43"/>
+      <c r="I122" s="43"/>
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
@@ -6144,9 +6277,9 @@
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
       <c r="E123" s="5"/>
-      <c r="G123" s="32"/>
-      <c r="H123" s="32"/>
-      <c r="I123" s="32"/>
+      <c r="G123" s="43"/>
+      <c r="H123" s="43"/>
+      <c r="I123" s="43"/>
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
@@ -6175,9 +6308,9 @@
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
-      <c r="G124" s="32"/>
-      <c r="H124" s="32"/>
-      <c r="I124" s="32"/>
+      <c r="G124" s="43"/>
+      <c r="H124" s="43"/>
+      <c r="I124" s="43"/>
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
@@ -6206,9 +6339,9 @@
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
       <c r="E125" s="5"/>
-      <c r="G125" s="32"/>
-      <c r="H125" s="32"/>
-      <c r="I125" s="32"/>
+      <c r="G125" s="43"/>
+      <c r="H125" s="43"/>
+      <c r="I125" s="43"/>
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
@@ -6237,9 +6370,9 @@
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
-      <c r="G126" s="32"/>
-      <c r="H126" s="32"/>
-      <c r="I126" s="32"/>
+      <c r="G126" s="43"/>
+      <c r="H126" s="43"/>
+      <c r="I126" s="43"/>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
@@ -6268,9 +6401,9 @@
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
-      <c r="G127" s="32"/>
-      <c r="H127" s="32"/>
-      <c r="I127" s="32"/>
+      <c r="G127" s="43"/>
+      <c r="H127" s="43"/>
+      <c r="I127" s="43"/>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
@@ -6299,9 +6432,9 @@
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
-      <c r="G128" s="32"/>
-      <c r="H128" s="32"/>
-      <c r="I128" s="32"/>
+      <c r="G128" s="43"/>
+      <c r="H128" s="43"/>
+      <c r="I128" s="43"/>
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
@@ -6330,9 +6463,9 @@
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
-      <c r="G129" s="32"/>
-      <c r="H129" s="32"/>
-      <c r="I129" s="32"/>
+      <c r="G129" s="43"/>
+      <c r="H129" s="43"/>
+      <c r="I129" s="43"/>
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
@@ -6361,9 +6494,9 @@
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
-      <c r="G130" s="32"/>
-      <c r="H130" s="32"/>
-      <c r="I130" s="32"/>
+      <c r="G130" s="43"/>
+      <c r="H130" s="43"/>
+      <c r="I130" s="43"/>
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
@@ -6392,9 +6525,9 @@
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
       <c r="E131" s="5"/>
-      <c r="G131" s="32"/>
-      <c r="H131" s="32"/>
-      <c r="I131" s="32"/>
+      <c r="G131" s="43"/>
+      <c r="H131" s="43"/>
+      <c r="I131" s="43"/>
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
@@ -6423,9 +6556,9 @@
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
       <c r="E132" s="5"/>
-      <c r="G132" s="32"/>
-      <c r="H132" s="32"/>
-      <c r="I132" s="32"/>
+      <c r="G132" s="43"/>
+      <c r="H132" s="43"/>
+      <c r="I132" s="43"/>
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
@@ -6454,9 +6587,9 @@
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
       <c r="E133" s="5"/>
-      <c r="G133" s="32"/>
-      <c r="H133" s="32"/>
-      <c r="I133" s="32"/>
+      <c r="G133" s="43"/>
+      <c r="H133" s="43"/>
+      <c r="I133" s="43"/>
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
@@ -6485,9 +6618,9 @@
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
       <c r="E134" s="5"/>
-      <c r="G134" s="32"/>
-      <c r="H134" s="32"/>
-      <c r="I134" s="32"/>
+      <c r="G134" s="43"/>
+      <c r="H134" s="43"/>
+      <c r="I134" s="43"/>
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
@@ -6516,9 +6649,9 @@
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
       <c r="E135" s="5"/>
-      <c r="G135" s="32"/>
-      <c r="H135" s="32"/>
-      <c r="I135" s="32"/>
+      <c r="G135" s="43"/>
+      <c r="H135" s="43"/>
+      <c r="I135" s="43"/>
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
@@ -6547,9 +6680,9 @@
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
       <c r="E136" s="5"/>
-      <c r="G136" s="32"/>
-      <c r="H136" s="32"/>
-      <c r="I136" s="32"/>
+      <c r="G136" s="43"/>
+      <c r="H136" s="43"/>
+      <c r="I136" s="43"/>
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
@@ -6578,9 +6711,9 @@
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
-      <c r="G137" s="32"/>
-      <c r="H137" s="32"/>
-      <c r="I137" s="32"/>
+      <c r="G137" s="43"/>
+      <c r="H137" s="43"/>
+      <c r="I137" s="43"/>
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
@@ -6609,9 +6742,9 @@
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
       <c r="E138" s="5"/>
-      <c r="G138" s="32"/>
-      <c r="H138" s="32"/>
-      <c r="I138" s="32"/>
+      <c r="G138" s="43"/>
+      <c r="H138" s="43"/>
+      <c r="I138" s="43"/>
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
@@ -6640,9 +6773,9 @@
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
       <c r="E139" s="5"/>
-      <c r="G139" s="32"/>
-      <c r="H139" s="32"/>
-      <c r="I139" s="32"/>
+      <c r="G139" s="43"/>
+      <c r="H139" s="43"/>
+      <c r="I139" s="43"/>
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
@@ -6671,9 +6804,9 @@
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
       <c r="E140" s="5"/>
-      <c r="G140" s="32"/>
-      <c r="H140" s="32"/>
-      <c r="I140" s="32"/>
+      <c r="G140" s="43"/>
+      <c r="H140" s="43"/>
+      <c r="I140" s="43"/>
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
@@ -6702,9 +6835,9 @@
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
       <c r="E141" s="5"/>
-      <c r="G141" s="32"/>
-      <c r="H141" s="32"/>
-      <c r="I141" s="32"/>
+      <c r="G141" s="43"/>
+      <c r="H141" s="43"/>
+      <c r="I141" s="43"/>
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
@@ -6733,9 +6866,9 @@
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
       <c r="E142" s="5"/>
-      <c r="G142" s="32"/>
-      <c r="H142" s="32"/>
-      <c r="I142" s="32"/>
+      <c r="G142" s="43"/>
+      <c r="H142" s="43"/>
+      <c r="I142" s="43"/>
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
@@ -6764,9 +6897,9 @@
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
       <c r="E143" s="5"/>
-      <c r="G143" s="32"/>
-      <c r="H143" s="32"/>
-      <c r="I143" s="32"/>
+      <c r="G143" s="43"/>
+      <c r="H143" s="43"/>
+      <c r="I143" s="43"/>
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
@@ -6795,9 +6928,9 @@
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
       <c r="E144" s="5"/>
-      <c r="G144" s="32"/>
-      <c r="H144" s="32"/>
-      <c r="I144" s="32"/>
+      <c r="G144" s="43"/>
+      <c r="H144" s="43"/>
+      <c r="I144" s="43"/>
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
@@ -6826,9 +6959,9 @@
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
-      <c r="G145" s="32"/>
-      <c r="H145" s="32"/>
-      <c r="I145" s="32"/>
+      <c r="G145" s="43"/>
+      <c r="H145" s="43"/>
+      <c r="I145" s="43"/>
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
@@ -6857,9 +6990,9 @@
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
-      <c r="G146" s="32"/>
-      <c r="H146" s="32"/>
-      <c r="I146" s="32"/>
+      <c r="G146" s="43"/>
+      <c r="H146" s="43"/>
+      <c r="I146" s="43"/>
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
@@ -6888,9 +7021,9 @@
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
-      <c r="G147" s="32"/>
-      <c r="H147" s="32"/>
-      <c r="I147" s="32"/>
+      <c r="G147" s="43"/>
+      <c r="H147" s="43"/>
+      <c r="I147" s="43"/>
       <c r="J147" s="1"/>
       <c r="K147" s="1"/>
       <c r="L147" s="1"/>
@@ -6919,9 +7052,9 @@
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
-      <c r="G148" s="32"/>
-      <c r="H148" s="32"/>
-      <c r="I148" s="32"/>
+      <c r="G148" s="43"/>
+      <c r="H148" s="43"/>
+      <c r="I148" s="43"/>
       <c r="J148" s="1"/>
       <c r="K148" s="1"/>
       <c r="L148" s="1"/>
@@ -6950,9 +7083,9 @@
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
       <c r="E149" s="5"/>
-      <c r="G149" s="32"/>
-      <c r="H149" s="32"/>
-      <c r="I149" s="32"/>
+      <c r="G149" s="43"/>
+      <c r="H149" s="43"/>
+      <c r="I149" s="43"/>
       <c r="J149" s="1"/>
       <c r="K149" s="1"/>
       <c r="L149" s="1"/>
@@ -6981,9 +7114,9 @@
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
       <c r="E150" s="5"/>
-      <c r="G150" s="32"/>
-      <c r="H150" s="32"/>
-      <c r="I150" s="32"/>
+      <c r="G150" s="43"/>
+      <c r="H150" s="43"/>
+      <c r="I150" s="43"/>
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
       <c r="L150" s="1"/>
@@ -7012,9 +7145,9 @@
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
       <c r="E151" s="5"/>
-      <c r="G151" s="32"/>
-      <c r="H151" s="32"/>
-      <c r="I151" s="32"/>
+      <c r="G151" s="43"/>
+      <c r="H151" s="43"/>
+      <c r="I151" s="43"/>
       <c r="J151" s="1"/>
       <c r="K151" s="1"/>
       <c r="L151" s="1"/>
@@ -7043,9 +7176,9 @@
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
       <c r="E152" s="5"/>
-      <c r="G152" s="32"/>
-      <c r="H152" s="32"/>
-      <c r="I152" s="32"/>
+      <c r="G152" s="43"/>
+      <c r="H152" s="43"/>
+      <c r="I152" s="43"/>
       <c r="J152" s="1"/>
       <c r="K152" s="1"/>
       <c r="L152" s="1"/>
@@ -7074,9 +7207,9 @@
       <c r="C153" s="5"/>
       <c r="D153" s="5"/>
       <c r="E153" s="5"/>
-      <c r="G153" s="32"/>
-      <c r="H153" s="32"/>
-      <c r="I153" s="32"/>
+      <c r="G153" s="43"/>
+      <c r="H153" s="43"/>
+      <c r="I153" s="43"/>
       <c r="J153" s="1"/>
       <c r="K153" s="1"/>
       <c r="L153" s="1"/>
@@ -7105,9 +7238,9 @@
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
       <c r="E154" s="5"/>
-      <c r="G154" s="32"/>
-      <c r="H154" s="32"/>
-      <c r="I154" s="32"/>
+      <c r="G154" s="43"/>
+      <c r="H154" s="43"/>
+      <c r="I154" s="43"/>
       <c r="J154" s="1"/>
       <c r="K154" s="1"/>
       <c r="L154" s="1"/>
@@ -7136,9 +7269,9 @@
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
       <c r="E155" s="5"/>
-      <c r="G155" s="32"/>
-      <c r="H155" s="32"/>
-      <c r="I155" s="32"/>
+      <c r="G155" s="43"/>
+      <c r="H155" s="43"/>
+      <c r="I155" s="43"/>
       <c r="J155" s="1"/>
       <c r="K155" s="1"/>
       <c r="L155" s="1"/>
@@ -7167,9 +7300,9 @@
       <c r="C156" s="5"/>
       <c r="D156" s="5"/>
       <c r="E156" s="5"/>
-      <c r="G156" s="32"/>
-      <c r="H156" s="32"/>
-      <c r="I156" s="32"/>
+      <c r="G156" s="43"/>
+      <c r="H156" s="43"/>
+      <c r="I156" s="43"/>
       <c r="J156" s="1"/>
       <c r="K156" s="1"/>
       <c r="L156" s="1"/>
@@ -7198,9 +7331,9 @@
       <c r="C157" s="5"/>
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
-      <c r="G157" s="32"/>
-      <c r="H157" s="32"/>
-      <c r="I157" s="32"/>
+      <c r="G157" s="43"/>
+      <c r="H157" s="43"/>
+      <c r="I157" s="43"/>
       <c r="J157" s="1"/>
       <c r="K157" s="1"/>
       <c r="L157" s="1"/>
@@ -7229,9 +7362,9 @@
       <c r="C158" s="5"/>
       <c r="D158" s="5"/>
       <c r="E158" s="5"/>
-      <c r="G158" s="32"/>
-      <c r="H158" s="32"/>
-      <c r="I158" s="32"/>
+      <c r="G158" s="43"/>
+      <c r="H158" s="43"/>
+      <c r="I158" s="43"/>
       <c r="J158" s="1"/>
       <c r="K158" s="1"/>
       <c r="L158" s="1"/>
@@ -7260,9 +7393,9 @@
       <c r="C159" s="5"/>
       <c r="D159" s="5"/>
       <c r="E159" s="5"/>
-      <c r="G159" s="32"/>
-      <c r="H159" s="32"/>
-      <c r="I159" s="32"/>
+      <c r="G159" s="43"/>
+      <c r="H159" s="43"/>
+      <c r="I159" s="43"/>
       <c r="J159" s="1"/>
       <c r="K159" s="1"/>
       <c r="L159" s="1"/>
@@ -7291,9 +7424,9 @@
       <c r="C160" s="5"/>
       <c r="D160" s="5"/>
       <c r="E160" s="5"/>
-      <c r="G160" s="32"/>
-      <c r="H160" s="32"/>
-      <c r="I160" s="32"/>
+      <c r="G160" s="43"/>
+      <c r="H160" s="43"/>
+      <c r="I160" s="43"/>
       <c r="J160" s="1"/>
       <c r="K160" s="1"/>
       <c r="L160" s="1"/>
@@ -7322,9 +7455,9 @@
       <c r="C161" s="5"/>
       <c r="D161" s="5"/>
       <c r="E161" s="5"/>
-      <c r="G161" s="32"/>
-      <c r="H161" s="32"/>
-      <c r="I161" s="32"/>
+      <c r="G161" s="43"/>
+      <c r="H161" s="43"/>
+      <c r="I161" s="43"/>
       <c r="J161" s="1"/>
       <c r="K161" s="1"/>
       <c r="L161" s="1"/>
@@ -7353,9 +7486,9 @@
       <c r="C162" s="5"/>
       <c r="D162" s="5"/>
       <c r="E162" s="5"/>
-      <c r="G162" s="32"/>
-      <c r="H162" s="32"/>
-      <c r="I162" s="32"/>
+      <c r="G162" s="43"/>
+      <c r="H162" s="43"/>
+      <c r="I162" s="43"/>
       <c r="J162" s="1"/>
       <c r="K162" s="1"/>
       <c r="L162" s="1"/>
@@ -7384,9 +7517,9 @@
       <c r="C163" s="5"/>
       <c r="D163" s="5"/>
       <c r="E163" s="5"/>
-      <c r="G163" s="32"/>
-      <c r="H163" s="32"/>
-      <c r="I163" s="32"/>
+      <c r="G163" s="43"/>
+      <c r="H163" s="43"/>
+      <c r="I163" s="43"/>
       <c r="J163" s="1"/>
       <c r="K163" s="1"/>
       <c r="L163" s="1"/>
@@ -7415,9 +7548,9 @@
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
-      <c r="G164" s="32"/>
-      <c r="H164" s="32"/>
-      <c r="I164" s="32"/>
+      <c r="G164" s="43"/>
+      <c r="H164" s="43"/>
+      <c r="I164" s="43"/>
       <c r="J164" s="1"/>
       <c r="K164" s="1"/>
       <c r="L164" s="1"/>
@@ -7446,9 +7579,9 @@
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
       <c r="E165" s="5"/>
-      <c r="G165" s="32"/>
-      <c r="H165" s="32"/>
-      <c r="I165" s="32"/>
+      <c r="G165" s="43"/>
+      <c r="H165" s="43"/>
+      <c r="I165" s="43"/>
       <c r="J165" s="1"/>
       <c r="K165" s="1"/>
       <c r="L165" s="1"/>
@@ -7477,9 +7610,9 @@
       <c r="C166" s="5"/>
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
-      <c r="G166" s="32"/>
-      <c r="H166" s="32"/>
-      <c r="I166" s="32"/>
+      <c r="G166" s="43"/>
+      <c r="H166" s="43"/>
+      <c r="I166" s="43"/>
       <c r="J166" s="1"/>
       <c r="K166" s="1"/>
       <c r="L166" s="1"/>
@@ -7508,9 +7641,9 @@
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
       <c r="E167" s="5"/>
-      <c r="G167" s="32"/>
-      <c r="H167" s="32"/>
-      <c r="I167" s="32"/>
+      <c r="G167" s="43"/>
+      <c r="H167" s="43"/>
+      <c r="I167" s="43"/>
       <c r="J167" s="1"/>
       <c r="K167" s="1"/>
       <c r="L167" s="1"/>
@@ -7539,9 +7672,9 @@
       <c r="C168" s="5"/>
       <c r="D168" s="5"/>
       <c r="E168" s="5"/>
-      <c r="G168" s="32"/>
-      <c r="H168" s="32"/>
-      <c r="I168" s="32"/>
+      <c r="G168" s="43"/>
+      <c r="H168" s="43"/>
+      <c r="I168" s="43"/>
       <c r="J168" s="1"/>
       <c r="K168" s="1"/>
       <c r="L168" s="1"/>
@@ -7570,9 +7703,9 @@
       <c r="C169" s="5"/>
       <c r="D169" s="5"/>
       <c r="E169" s="5"/>
-      <c r="G169" s="32"/>
-      <c r="H169" s="32"/>
-      <c r="I169" s="32"/>
+      <c r="G169" s="43"/>
+      <c r="H169" s="43"/>
+      <c r="I169" s="43"/>
       <c r="J169" s="1"/>
       <c r="K169" s="1"/>
       <c r="L169" s="1"/>
@@ -7601,9 +7734,9 @@
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
       <c r="E170" s="5"/>
-      <c r="G170" s="32"/>
-      <c r="H170" s="32"/>
-      <c r="I170" s="32"/>
+      <c r="G170" s="43"/>
+      <c r="H170" s="43"/>
+      <c r="I170" s="43"/>
       <c r="J170" s="1"/>
       <c r="K170" s="1"/>
       <c r="L170" s="1"/>
@@ -7632,9 +7765,9 @@
       <c r="C171" s="5"/>
       <c r="D171" s="5"/>
       <c r="E171" s="5"/>
-      <c r="G171" s="32"/>
-      <c r="H171" s="32"/>
-      <c r="I171" s="32"/>
+      <c r="G171" s="43"/>
+      <c r="H171" s="43"/>
+      <c r="I171" s="43"/>
       <c r="J171" s="1"/>
       <c r="K171" s="1"/>
       <c r="L171" s="1"/>
@@ -7663,9 +7796,9 @@
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
       <c r="E172" s="5"/>
-      <c r="G172" s="32"/>
-      <c r="H172" s="32"/>
-      <c r="I172" s="32"/>
+      <c r="G172" s="43"/>
+      <c r="H172" s="43"/>
+      <c r="I172" s="43"/>
       <c r="J172" s="1"/>
       <c r="K172" s="1"/>
       <c r="L172" s="1"/>
@@ -7694,9 +7827,9 @@
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
-      <c r="G173" s="32"/>
-      <c r="H173" s="32"/>
-      <c r="I173" s="32"/>
+      <c r="G173" s="43"/>
+      <c r="H173" s="43"/>
+      <c r="I173" s="43"/>
       <c r="J173" s="1"/>
       <c r="K173" s="1"/>
       <c r="L173" s="1"/>
@@ -7725,9 +7858,9 @@
       <c r="C174" s="5"/>
       <c r="D174" s="5"/>
       <c r="E174" s="5"/>
-      <c r="G174" s="32"/>
-      <c r="H174" s="32"/>
-      <c r="I174" s="32"/>
+      <c r="G174" s="43"/>
+      <c r="H174" s="43"/>
+      <c r="I174" s="43"/>
       <c r="J174" s="1"/>
       <c r="K174" s="1"/>
       <c r="L174" s="1"/>
@@ -7756,9 +7889,9 @@
       <c r="C175" s="5"/>
       <c r="D175" s="5"/>
       <c r="E175" s="5"/>
-      <c r="G175" s="32"/>
-      <c r="H175" s="32"/>
-      <c r="I175" s="32"/>
+      <c r="G175" s="43"/>
+      <c r="H175" s="43"/>
+      <c r="I175" s="43"/>
       <c r="J175" s="1"/>
       <c r="K175" s="1"/>
       <c r="L175" s="1"/>
@@ -7787,9 +7920,9 @@
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
       <c r="E176" s="5"/>
-      <c r="G176" s="32"/>
-      <c r="H176" s="32"/>
-      <c r="I176" s="32"/>
+      <c r="G176" s="43"/>
+      <c r="H176" s="43"/>
+      <c r="I176" s="43"/>
       <c r="J176" s="1"/>
       <c r="K176" s="1"/>
       <c r="L176" s="1"/>
@@ -7818,9 +7951,9 @@
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
       <c r="E177" s="5"/>
-      <c r="G177" s="32"/>
-      <c r="H177" s="32"/>
-      <c r="I177" s="32"/>
+      <c r="G177" s="43"/>
+      <c r="H177" s="43"/>
+      <c r="I177" s="43"/>
       <c r="J177" s="1"/>
       <c r="K177" s="1"/>
       <c r="L177" s="1"/>
@@ -7849,9 +7982,9 @@
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
       <c r="E178" s="5"/>
-      <c r="G178" s="32"/>
-      <c r="H178" s="32"/>
-      <c r="I178" s="32"/>
+      <c r="G178" s="43"/>
+      <c r="H178" s="43"/>
+      <c r="I178" s="43"/>
       <c r="J178" s="1"/>
       <c r="K178" s="1"/>
       <c r="L178" s="1"/>
@@ -7880,9 +8013,9 @@
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
       <c r="E179" s="5"/>
-      <c r="G179" s="32"/>
-      <c r="H179" s="32"/>
-      <c r="I179" s="32"/>
+      <c r="G179" s="43"/>
+      <c r="H179" s="43"/>
+      <c r="I179" s="43"/>
       <c r="J179" s="1"/>
       <c r="K179" s="1"/>
       <c r="L179" s="1"/>
@@ -7911,9 +8044,9 @@
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
       <c r="E180" s="5"/>
-      <c r="G180" s="32"/>
-      <c r="H180" s="32"/>
-      <c r="I180" s="32"/>
+      <c r="G180" s="43"/>
+      <c r="H180" s="43"/>
+      <c r="I180" s="43"/>
       <c r="J180" s="1"/>
       <c r="K180" s="1"/>
       <c r="L180" s="1"/>
@@ -7942,9 +8075,9 @@
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
       <c r="E181" s="5"/>
-      <c r="G181" s="32"/>
-      <c r="H181" s="32"/>
-      <c r="I181" s="32"/>
+      <c r="G181" s="43"/>
+      <c r="H181" s="43"/>
+      <c r="I181" s="43"/>
       <c r="J181" s="1"/>
       <c r="K181" s="1"/>
       <c r="L181" s="1"/>
@@ -7973,9 +8106,9 @@
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
       <c r="E182" s="5"/>
-      <c r="G182" s="32"/>
-      <c r="H182" s="32"/>
-      <c r="I182" s="32"/>
+      <c r="G182" s="43"/>
+      <c r="H182" s="43"/>
+      <c r="I182" s="43"/>
       <c r="J182" s="1"/>
       <c r="K182" s="1"/>
       <c r="L182" s="1"/>
@@ -8004,9 +8137,9 @@
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
       <c r="E183" s="5"/>
-      <c r="G183" s="32"/>
-      <c r="H183" s="32"/>
-      <c r="I183" s="32"/>
+      <c r="G183" s="43"/>
+      <c r="H183" s="43"/>
+      <c r="I183" s="43"/>
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
       <c r="L183" s="1"/>
@@ -8035,9 +8168,9 @@
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
       <c r="E184" s="5"/>
-      <c r="G184" s="32"/>
-      <c r="H184" s="32"/>
-      <c r="I184" s="32"/>
+      <c r="G184" s="43"/>
+      <c r="H184" s="43"/>
+      <c r="I184" s="43"/>
       <c r="J184" s="1"/>
       <c r="K184" s="1"/>
       <c r="L184" s="1"/>
@@ -8066,9 +8199,9 @@
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
       <c r="E185" s="5"/>
-      <c r="G185" s="32"/>
-      <c r="H185" s="32"/>
-      <c r="I185" s="32"/>
+      <c r="G185" s="43"/>
+      <c r="H185" s="43"/>
+      <c r="I185" s="43"/>
       <c r="J185" s="1"/>
       <c r="K185" s="1"/>
       <c r="L185" s="1"/>
@@ -8097,9 +8230,9 @@
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
       <c r="E186" s="5"/>
-      <c r="G186" s="32"/>
-      <c r="H186" s="32"/>
-      <c r="I186" s="32"/>
+      <c r="G186" s="43"/>
+      <c r="H186" s="43"/>
+      <c r="I186" s="43"/>
       <c r="J186" s="1"/>
       <c r="K186" s="1"/>
       <c r="L186" s="1"/>
@@ -8128,9 +8261,9 @@
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
       <c r="E187" s="5"/>
-      <c r="G187" s="32"/>
-      <c r="H187" s="32"/>
-      <c r="I187" s="32"/>
+      <c r="G187" s="43"/>
+      <c r="H187" s="43"/>
+      <c r="I187" s="43"/>
       <c r="J187" s="1"/>
       <c r="K187" s="1"/>
       <c r="L187" s="1"/>
@@ -8159,9 +8292,9 @@
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
       <c r="E188" s="5"/>
-      <c r="G188" s="32"/>
-      <c r="H188" s="32"/>
-      <c r="I188" s="32"/>
+      <c r="G188" s="43"/>
+      <c r="H188" s="43"/>
+      <c r="I188" s="43"/>
       <c r="J188" s="1"/>
       <c r="K188" s="1"/>
       <c r="L188" s="1"/>
@@ -8190,9 +8323,9 @@
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
       <c r="E189" s="5"/>
-      <c r="G189" s="32"/>
-      <c r="H189" s="32"/>
-      <c r="I189" s="32"/>
+      <c r="G189" s="43"/>
+      <c r="H189" s="43"/>
+      <c r="I189" s="43"/>
       <c r="J189" s="1"/>
       <c r="K189" s="1"/>
       <c r="L189" s="1"/>
@@ -8221,9 +8354,9 @@
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
       <c r="E190" s="5"/>
-      <c r="G190" s="32"/>
-      <c r="H190" s="32"/>
-      <c r="I190" s="32"/>
+      <c r="G190" s="43"/>
+      <c r="H190" s="43"/>
+      <c r="I190" s="43"/>
       <c r="J190" s="1"/>
       <c r="K190" s="1"/>
       <c r="L190" s="1"/>
@@ -8252,9 +8385,9 @@
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
       <c r="E191" s="5"/>
-      <c r="G191" s="32"/>
-      <c r="H191" s="32"/>
-      <c r="I191" s="32"/>
+      <c r="G191" s="43"/>
+      <c r="H191" s="43"/>
+      <c r="I191" s="43"/>
       <c r="J191" s="1"/>
       <c r="K191" s="1"/>
       <c r="L191" s="1"/>
@@ -8283,9 +8416,9 @@
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
       <c r="E192" s="5"/>
-      <c r="G192" s="32"/>
-      <c r="H192" s="32"/>
-      <c r="I192" s="32"/>
+      <c r="G192" s="43"/>
+      <c r="H192" s="43"/>
+      <c r="I192" s="43"/>
       <c r="J192" s="1"/>
       <c r="K192" s="1"/>
       <c r="L192" s="1"/>
@@ -8314,9 +8447,9 @@
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
       <c r="E193" s="5"/>
-      <c r="G193" s="32"/>
-      <c r="H193" s="32"/>
-      <c r="I193" s="32"/>
+      <c r="G193" s="43"/>
+      <c r="H193" s="43"/>
+      <c r="I193" s="43"/>
       <c r="J193" s="1"/>
       <c r="K193" s="1"/>
       <c r="L193" s="1"/>
@@ -8345,9 +8478,9 @@
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
       <c r="E194" s="5"/>
-      <c r="G194" s="32"/>
-      <c r="H194" s="32"/>
-      <c r="I194" s="32"/>
+      <c r="G194" s="43"/>
+      <c r="H194" s="43"/>
+      <c r="I194" s="43"/>
       <c r="J194" s="1"/>
       <c r="K194" s="1"/>
       <c r="L194" s="1"/>
@@ -8376,9 +8509,9 @@
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
       <c r="E195" s="5"/>
-      <c r="G195" s="32"/>
-      <c r="H195" s="32"/>
-      <c r="I195" s="32"/>
+      <c r="G195" s="43"/>
+      <c r="H195" s="43"/>
+      <c r="I195" s="43"/>
       <c r="J195" s="1"/>
       <c r="K195" s="1"/>
       <c r="L195" s="1"/>
@@ -8407,9 +8540,9 @@
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
       <c r="E196" s="5"/>
-      <c r="G196" s="32"/>
-      <c r="H196" s="32"/>
-      <c r="I196" s="32"/>
+      <c r="G196" s="43"/>
+      <c r="H196" s="43"/>
+      <c r="I196" s="43"/>
       <c r="J196" s="1"/>
       <c r="K196" s="1"/>
       <c r="L196" s="1"/>
@@ -8438,9 +8571,9 @@
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
       <c r="E197" s="5"/>
-      <c r="G197" s="32"/>
-      <c r="H197" s="32"/>
-      <c r="I197" s="32"/>
+      <c r="G197" s="43"/>
+      <c r="H197" s="43"/>
+      <c r="I197" s="43"/>
       <c r="J197" s="1"/>
       <c r="K197" s="1"/>
       <c r="L197" s="1"/>
@@ -8469,9 +8602,9 @@
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
       <c r="E198" s="5"/>
-      <c r="G198" s="32"/>
-      <c r="H198" s="32"/>
-      <c r="I198" s="32"/>
+      <c r="G198" s="43"/>
+      <c r="H198" s="43"/>
+      <c r="I198" s="43"/>
       <c r="J198" s="1"/>
       <c r="K198" s="1"/>
       <c r="L198" s="1"/>
@@ -8500,9 +8633,9 @@
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
       <c r="E199" s="5"/>
-      <c r="G199" s="32"/>
-      <c r="H199" s="32"/>
-      <c r="I199" s="32"/>
+      <c r="G199" s="43"/>
+      <c r="H199" s="43"/>
+      <c r="I199" s="43"/>
       <c r="J199" s="1"/>
       <c r="K199" s="1"/>
       <c r="L199" s="1"/>
@@ -8531,9 +8664,9 @@
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
       <c r="E200" s="5"/>
-      <c r="G200" s="32"/>
-      <c r="H200" s="32"/>
-      <c r="I200" s="32"/>
+      <c r="G200" s="43"/>
+      <c r="H200" s="43"/>
+      <c r="I200" s="43"/>
       <c r="J200" s="1"/>
       <c r="K200" s="1"/>
       <c r="L200" s="1"/>
@@ -8562,9 +8695,9 @@
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
       <c r="E201" s="5"/>
-      <c r="G201" s="32"/>
-      <c r="H201" s="32"/>
-      <c r="I201" s="32"/>
+      <c r="G201" s="43"/>
+      <c r="H201" s="43"/>
+      <c r="I201" s="43"/>
       <c r="J201" s="1"/>
       <c r="K201" s="1"/>
       <c r="L201" s="1"/>
@@ -8593,9 +8726,9 @@
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
       <c r="E202" s="5"/>
-      <c r="G202" s="32"/>
-      <c r="H202" s="32"/>
-      <c r="I202" s="32"/>
+      <c r="G202" s="43"/>
+      <c r="H202" s="43"/>
+      <c r="I202" s="43"/>
       <c r="J202" s="1"/>
       <c r="K202" s="1"/>
       <c r="L202" s="1"/>
@@ -8624,9 +8757,9 @@
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
       <c r="E203" s="5"/>
-      <c r="G203" s="32"/>
-      <c r="H203" s="32"/>
-      <c r="I203" s="32"/>
+      <c r="G203" s="43"/>
+      <c r="H203" s="43"/>
+      <c r="I203" s="43"/>
       <c r="J203" s="1"/>
       <c r="K203" s="1"/>
       <c r="L203" s="1"/>
@@ -8655,9 +8788,9 @@
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
       <c r="E204" s="5"/>
-      <c r="G204" s="32"/>
-      <c r="H204" s="32"/>
-      <c r="I204" s="32"/>
+      <c r="G204" s="43"/>
+      <c r="H204" s="43"/>
+      <c r="I204" s="43"/>
       <c r="J204" s="1"/>
       <c r="K204" s="1"/>
       <c r="L204" s="1"/>
@@ -8686,9 +8819,9 @@
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
       <c r="E205" s="5"/>
-      <c r="G205" s="32"/>
-      <c r="H205" s="32"/>
-      <c r="I205" s="32"/>
+      <c r="G205" s="43"/>
+      <c r="H205" s="43"/>
+      <c r="I205" s="43"/>
       <c r="J205" s="1"/>
       <c r="K205" s="1"/>
       <c r="L205" s="1"/>
@@ -8717,9 +8850,9 @@
       <c r="C206" s="5"/>
       <c r="D206" s="5"/>
       <c r="E206" s="5"/>
-      <c r="G206" s="32"/>
-      <c r="H206" s="32"/>
-      <c r="I206" s="32"/>
+      <c r="G206" s="43"/>
+      <c r="H206" s="43"/>
+      <c r="I206" s="43"/>
       <c r="J206" s="1"/>
       <c r="K206" s="1"/>
       <c r="L206" s="1"/>
@@ -8748,9 +8881,9 @@
       <c r="C207" s="5"/>
       <c r="D207" s="5"/>
       <c r="E207" s="5"/>
-      <c r="G207" s="32"/>
-      <c r="H207" s="32"/>
-      <c r="I207" s="32"/>
+      <c r="G207" s="43"/>
+      <c r="H207" s="43"/>
+      <c r="I207" s="43"/>
       <c r="J207" s="1"/>
       <c r="K207" s="1"/>
       <c r="L207" s="1"/>
@@ -8779,9 +8912,9 @@
       <c r="C208" s="5"/>
       <c r="D208" s="5"/>
       <c r="E208" s="5"/>
-      <c r="G208" s="32"/>
-      <c r="H208" s="32"/>
-      <c r="I208" s="32"/>
+      <c r="G208" s="43"/>
+      <c r="H208" s="43"/>
+      <c r="I208" s="43"/>
       <c r="J208" s="1"/>
       <c r="K208" s="1"/>
       <c r="L208" s="1"/>
@@ -8810,9 +8943,9 @@
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
       <c r="E209" s="5"/>
-      <c r="G209" s="32"/>
-      <c r="H209" s="32"/>
-      <c r="I209" s="32"/>
+      <c r="G209" s="43"/>
+      <c r="H209" s="43"/>
+      <c r="I209" s="43"/>
       <c r="J209" s="1"/>
       <c r="K209" s="1"/>
       <c r="L209" s="1"/>
@@ -8841,9 +8974,9 @@
       <c r="C210" s="5"/>
       <c r="D210" s="5"/>
       <c r="E210" s="5"/>
-      <c r="G210" s="32"/>
-      <c r="H210" s="32"/>
-      <c r="I210" s="32"/>
+      <c r="G210" s="43"/>
+      <c r="H210" s="43"/>
+      <c r="I210" s="43"/>
       <c r="J210" s="1"/>
       <c r="K210" s="1"/>
       <c r="L210" s="1"/>
@@ -8872,9 +9005,9 @@
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
       <c r="E211" s="5"/>
-      <c r="G211" s="32"/>
-      <c r="H211" s="32"/>
-      <c r="I211" s="32"/>
+      <c r="G211" s="43"/>
+      <c r="H211" s="43"/>
+      <c r="I211" s="43"/>
       <c r="J211" s="1"/>
       <c r="K211" s="1"/>
       <c r="L211" s="1"/>
@@ -8903,9 +9036,9 @@
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
       <c r="E212" s="5"/>
-      <c r="G212" s="32"/>
-      <c r="H212" s="32"/>
-      <c r="I212" s="32"/>
+      <c r="G212" s="43"/>
+      <c r="H212" s="43"/>
+      <c r="I212" s="43"/>
       <c r="J212" s="1"/>
       <c r="K212" s="1"/>
       <c r="L212" s="1"/>
@@ -8934,9 +9067,9 @@
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
       <c r="E213" s="5"/>
-      <c r="G213" s="32"/>
-      <c r="H213" s="32"/>
-      <c r="I213" s="32"/>
+      <c r="G213" s="43"/>
+      <c r="H213" s="43"/>
+      <c r="I213" s="43"/>
       <c r="J213" s="1"/>
       <c r="K213" s="1"/>
       <c r="L213" s="1"/>
@@ -8965,9 +9098,9 @@
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>
       <c r="E214" s="5"/>
-      <c r="G214" s="32"/>
-      <c r="H214" s="32"/>
-      <c r="I214" s="32"/>
+      <c r="G214" s="43"/>
+      <c r="H214" s="43"/>
+      <c r="I214" s="43"/>
       <c r="J214" s="1"/>
       <c r="K214" s="1"/>
       <c r="L214" s="1"/>
@@ -8996,9 +9129,9 @@
       <c r="C215" s="5"/>
       <c r="D215" s="5"/>
       <c r="E215" s="5"/>
-      <c r="G215" s="32"/>
-      <c r="H215" s="32"/>
-      <c r="I215" s="32"/>
+      <c r="G215" s="43"/>
+      <c r="H215" s="43"/>
+      <c r="I215" s="43"/>
       <c r="J215" s="1"/>
       <c r="K215" s="1"/>
       <c r="L215" s="1"/>
@@ -9027,9 +9160,9 @@
       <c r="C216" s="5"/>
       <c r="D216" s="5"/>
       <c r="E216" s="5"/>
-      <c r="G216" s="32"/>
-      <c r="H216" s="32"/>
-      <c r="I216" s="32"/>
+      <c r="G216" s="43"/>
+      <c r="H216" s="43"/>
+      <c r="I216" s="43"/>
       <c r="J216" s="1"/>
       <c r="K216" s="1"/>
       <c r="L216" s="1"/>
@@ -9058,9 +9191,9 @@
       <c r="C217" s="5"/>
       <c r="D217" s="5"/>
       <c r="E217" s="5"/>
-      <c r="G217" s="32"/>
-      <c r="H217" s="32"/>
-      <c r="I217" s="32"/>
+      <c r="G217" s="43"/>
+      <c r="H217" s="43"/>
+      <c r="I217" s="43"/>
       <c r="J217" s="1"/>
       <c r="K217" s="1"/>
       <c r="L217" s="1"/>
@@ -9089,9 +9222,9 @@
       <c r="C218" s="5"/>
       <c r="D218" s="5"/>
       <c r="E218" s="5"/>
-      <c r="G218" s="32"/>
-      <c r="H218" s="32"/>
-      <c r="I218" s="32"/>
+      <c r="G218" s="43"/>
+      <c r="H218" s="43"/>
+      <c r="I218" s="43"/>
       <c r="J218" s="1"/>
       <c r="K218" s="1"/>
       <c r="L218" s="1"/>
@@ -9120,9 +9253,9 @@
       <c r="C219" s="5"/>
       <c r="D219" s="5"/>
       <c r="E219" s="5"/>
-      <c r="G219" s="32"/>
-      <c r="H219" s="32"/>
-      <c r="I219" s="32"/>
+      <c r="G219" s="43"/>
+      <c r="H219" s="43"/>
+      <c r="I219" s="43"/>
       <c r="J219" s="1"/>
       <c r="K219" s="1"/>
       <c r="L219" s="1"/>
@@ -9151,9 +9284,9 @@
       <c r="C220" s="5"/>
       <c r="D220" s="5"/>
       <c r="E220" s="5"/>
-      <c r="G220" s="32"/>
-      <c r="H220" s="32"/>
-      <c r="I220" s="32"/>
+      <c r="G220" s="43"/>
+      <c r="H220" s="43"/>
+      <c r="I220" s="43"/>
       <c r="J220" s="1"/>
       <c r="K220" s="1"/>
       <c r="L220" s="1"/>

</xml_diff>